<commit_message>
edit dataBase detail for Snack App
</commit_message>
<xml_diff>
--- a/Snack ver1.3/データベース定義書.xlsx
+++ b/Snack ver1.3/データベース定義書.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217F6CF3-90C8-450F-9BF0-1C64B11BA0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21388292-9E4B-4870-9A01-5D3FF0A5700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="860" windowWidth="16050" windowHeight="8320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="18260" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -995,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -1008,7 +1008,7 @@
     <col min="6" max="7" width="5.1796875" customWidth="1"/>
     <col min="8" max="8" width="6.1796875" customWidth="1"/>
     <col min="9" max="9" width="21.453125" customWidth="1"/>
-    <col min="10" max="10" width="53.90625" customWidth="1"/>
+    <col min="10" max="10" width="34.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.3">
@@ -1819,6 +1819,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>